<commit_message>
Add column keterangan and set style column
</commit_message>
<xml_diff>
--- a/public/form/form-data-rekap-hasil-tes.xlsx
+++ b/public/form/form-data-rekap-hasil-tes.xlsx
@@ -34,13 +34,13 @@
     <t>Jumlah Tes</t>
   </si>
   <si>
-    <t>Tes</t>
-  </si>
-  <si>
     <t>DAFTAR NAMA TES</t>
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Keterangan</t>
   </si>
 </sst>
 </file>
@@ -86,7 +86,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -146,11 +146,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -194,6 +220,12 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -502,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU8"/>
+  <dimension ref="A1:AV8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,40 +545,41 @@
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="2" width="34.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="4" customWidth="1"/>
-    <col min="5" max="47" width="12.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="4" customWidth="1"/>
+    <col min="6" max="48" width="12.42578125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="10"/>
-      <c r="D5" s="11" t="s">
-        <v>6</v>
-      </c>
+      <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:47" s="9" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" s="9" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -556,14 +589,16 @@
       <c r="C7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="8"/>
+      <c r="F7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="15"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -604,14 +639,15 @@
       <c r="AS7" s="8"/>
       <c r="AT7" s="8"/>
       <c r="AU7" s="8"/>
+      <c r="AV7" s="8"/>
     </row>
-    <row r="8" spans="1:47" s="5" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" s="5" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="6"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="7"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -653,16 +689,18 @@
       <c r="AS8" s="6"/>
       <c r="AT8" s="6"/>
       <c r="AU8" s="6"/>
+      <c r="AV8" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="F7:G7"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="E7:F7"/>
   </mergeCells>
-  <conditionalFormatting sqref="D9:D634">
+  <conditionalFormatting sqref="E9:E634">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add field Username Export Rekap Hasil Tes
</commit_message>
<xml_diff>
--- a/public/form/form-data-rekap-hasil-tes.xlsx
+++ b/public/form/form-data-rekap-hasil-tes.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\tesonline\public\form\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B56AC3-A877-40C5-BEBD-7F335A4B4DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="19935" windowHeight="8130"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>No</t>
   </si>
@@ -41,12 +47,15 @@
   </si>
   <si>
     <t>Keterangan</t>
+  </si>
+  <si>
+    <t>Username</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -243,6 +252,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -290,7 +302,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -323,9 +335,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -358,6 +387,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -533,73 +579,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AW8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="4" customWidth="1"/>
-    <col min="6" max="48" width="12.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="4" customWidth="1"/>
+    <col min="7" max="49" width="12.42578125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="B1" s="3"/>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="B3" s="2"/>
       <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="B4" s="2"/>
       <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
+      <c r="B5" s="2"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:48" s="9" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" s="9" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="D7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="E7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="G7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="8"/>
+      <c r="H7" s="15"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -640,15 +694,16 @@
       <c r="AT7" s="8"/>
       <c r="AU7" s="8"/>
       <c r="AV7" s="8"/>
+      <c r="AW7" s="8"/>
     </row>
-    <row r="8" spans="1:48" s="5" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" s="5" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="12"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="6"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="7"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
@@ -690,17 +745,19 @@
       <c r="AT8" s="6"/>
       <c r="AU8" s="6"/>
       <c r="AV8" s="6"/>
+      <c r="AW8" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="E7:E8"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E9:E634">
+  <conditionalFormatting sqref="F9:F634">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add field Username Export Rekap Hasil Tes Rev2
</commit_message>
<xml_diff>
--- a/public/form/form-data-rekap-hasil-tes.xlsx
+++ b/public/form/form-data-rekap-hasil-tes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\tesonline\public\form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B56AC3-A877-40C5-BEBD-7F335A4B4DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FB5533-B208-4AE2-AC4A-E5A718DC85DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -580,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW8"/>
+  <dimension ref="A1:AW9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,6 +747,9 @@
       <c r="AV8" s="6"/>
       <c r="AW8" s="6"/>
     </row>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="C7:C8"/>

</xml_diff>

<commit_message>
Add field Username Export Rekap Hasil Tes Align left all row
</commit_message>
<xml_diff>
--- a/public/form/form-data-rekap-hasil-tes.xlsx
+++ b/public/form/form-data-rekap-hasil-tes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\tesonline\public\form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FB5533-B208-4AE2-AC4A-E5A718DC85DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC5506F-AF8B-4A21-BE20-0DA0A314B45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -185,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -235,6 +235,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,16 +583,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW9"/>
+  <dimension ref="A1:AW8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A1048539" workbookViewId="0">
+      <selection activeCell="C1048554" sqref="C1048554"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="18" customWidth="1"/>
     <col min="3" max="3" width="34.5703125" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
     <col min="5" max="5" width="23.140625" customWidth="1"/>
@@ -602,6 +605,9 @@
         <v>2</v>
       </c>
       <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -747,9 +753,6 @@
       <c r="AV8" s="6"/>
       <c r="AW8" s="6"/>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="C7:C8"/>

</xml_diff>